<commit_message>
Update CR and CR Review
</commit_message>
<xml_diff>
--- a/Input Documents/CR/PO_SAG_CR_ES_Review_Template.xlsx
+++ b/Input Documents/CR/PO_SAG_CR_ES_Review_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship\SAG\WEB_SWProcess_Documents\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E content\Graduation Project\Input Documents\ES_SWProcess_Documents\Input Documents\CR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BC5620-FF1D-46BD-8BF2-6ECB05CB3BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Entry Date</t>
   </si>
@@ -46,12 +47,51 @@
   </si>
   <si>
     <t>Proposed Solution</t>
+  </si>
+  <si>
+    <t>CR_REVIEW_001</t>
+  </si>
+  <si>
+    <t>17/10</t>
+  </si>
+  <si>
+    <t>Jana Muhammed</t>
+  </si>
+  <si>
+    <t>V1.2</t>
+  </si>
+  <si>
+    <t>1//Document Title</t>
+  </si>
+  <si>
+    <t>Document Title doesn't match the document's name</t>
+  </si>
+  <si>
+    <t>Document Title should be changed to ("PO_SAG_CR_Glasses")</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>CR_REVIEW_002</t>
+  </si>
+  <si>
+    <t>Reham Essam</t>
+  </si>
+  <si>
+    <t>1//Document Status/Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the author's name isn't the same as the last name in the document history table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The author's name should be changed to the latest author's name </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
@@ -135,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,34 +192,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -413,14 +433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -429,7 +449,7 @@
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="7" width="44.5546875" customWidth="1"/>
+    <col min="6" max="7" width="70.77734375" customWidth="1"/>
     <col min="8" max="8" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -460,27 +480,55 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -558,17 +606,17 @@
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A2:H9">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:H9">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>